<commit_message>
Invoice has been Fixed
</commit_message>
<xml_diff>
--- a/TestProject1/Data/TestData_Invoice.xlsx
+++ b/TestProject1/Data/TestData_Invoice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Bảo đảm chất lượng PM\reup-demoheotelbooking\TestProject1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1371E1-4D20-4B6C-A5A2-DE4621A5514E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79B4D0-600B-4910-BF36-CADC974998F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20550" windowHeight="15270" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BookingList" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
   <si>
     <t>BookingId</t>
   </si>
@@ -88,12 +88,21 @@
     <t>Success - Thanh toán tiền mặt thành công</t>
   </si>
   <si>
+    <t>http://localhost:5145/Invoice/InvoiceDetail/2?message=Thanh%20to%C3%A1n%20th%C3%A0nh%20c%C3%B4ng</t>
+  </si>
+  <si>
     <t>test-payment.momo.vn</t>
   </si>
   <si>
     <t>Success - Chuyển hướng đến MoMo</t>
   </si>
   <si>
+    <t>https://test-payment.momo.vn/v2/gateway/pay?t=TU9NT3w2Mzg3NzQ1NTM1NDE3NTQ0NjI&amp;s=7e00aad292c54c748e9e0570ae8e1926da76880d4cb7e133caa7b09a0d2ae9c7</t>
+  </si>
+  <si>
+    <t>Success - Chuyển hướng đến MoMo thành công</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -115,43 +124,28 @@
     <t>Thành Trung</t>
   </si>
   <si>
-    <t>0123456789</t>
+    <t>0123456781</t>
   </si>
   <si>
     <t>BOOKING LIST</t>
   </si>
   <si>
+    <t>CHECKIN</t>
+  </si>
+  <si>
+    <t>CHECKOUT</t>
+  </si>
+  <si>
+    <t>PAYMENT</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>/Invoice/InvoiceDetail/1</t>
+  </si>
+  <si>
     <t>/Invoice/BookingDetails/1</t>
-  </si>
-  <si>
-    <t>CHECKIN</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>CHECKOUT</t>
-  </si>
-  <si>
-    <t>PAYMENT</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>/Invoice/InvoiceDetail/1</t>
-  </si>
-  <si>
-    <t>http://localhost:5145/Invoice/InvoiceDetail/1?message=Thanh%20to%C3%A1n%20th%C3%A0nh%20c%C3%B4ng</t>
-  </si>
-  <si>
-    <t>http://localhost:5145/Invoice/InvoiceDetail/2?message=Thanh%20to%C3%A1n%20th%C3%A0nh%20c%C3%B4ng</t>
-  </si>
-  <si>
-    <t>https://test-payment.momo.vn/v2/gateway/pay?t=TU9NT3w2Mzg3NzQ1NTM1NDE3NTQ0NjI&amp;s=7e00aad292c54c748e9e0570ae8e1926da76880d4cb7e133caa7b09a0d2ae9c7</t>
-  </si>
-  <si>
-    <t>Success - Chuyển hướng đến MoMo thành công</t>
   </si>
 </sst>
 </file>
@@ -894,7 +888,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>18</v>
@@ -911,16 +905,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>7</v>
@@ -1007,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31194945-AB3C-458B-BF0A-62250E40CDA8}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1026,19 +1020,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>2</v>
@@ -1050,15 +1044,15 @@
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C2" s="13">
         <v>45963</v>
@@ -1067,17 +1061,13 @@
         <v>45993</v>
       </c>
       <c r="E2" s="15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9">
@@ -1100,7 +1090,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1108,11 +1098,9 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="9"/>
       <c r="F5" s="2"/>
@@ -1131,22 +1119,18 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="9" t="s">
-        <v>32</v>
+      <c r="A8" s="9">
+        <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="1"/>
     </row>
     <row r="11" spans="1:9">
@@ -1163,22 +1147,18 @@
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="7" t="s">
-        <v>32</v>
+      <c r="A12" s="7">
+        <v>1</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="2"/>
     </row>
     <row r="15" spans="1:9">
@@ -1204,31 +1184,25 @@
         <v>4</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>32</v>
+      <c r="A16" s="7">
+        <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="1"/>
     </row>
   </sheetData>

</xml_diff>